<commit_message>
Build site at 2021-02-05 20:12:25 UTC
</commit_message>
<xml_diff>
--- a/assets/cursos/EM/docentes-EM.xlsx
+++ b/assets/cursos/EM/docentes-EM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="319">
   <si>
     <t>EM</t>
   </si>
@@ -307,6 +307,12 @@
     <t xml:space="preserve"> Diagrama de Fases</t>
   </si>
   <si>
+    <t>5009972</t>
+  </si>
+  <si>
+    <t>Gilberto Carvalho Coelho</t>
+  </si>
+  <si>
     <t>LOM3006</t>
   </si>
   <si>
@@ -391,6 +397,12 @@
     <t xml:space="preserve"> Termodinâmica de Materiais</t>
   </si>
   <si>
+    <t>1176388</t>
+  </si>
+  <si>
+    <t>Luiz Tadeu Fernandes Eleno</t>
+  </si>
+  <si>
     <t>LOM3018</t>
   </si>
   <si>
@@ -583,12 +595,6 @@
     <t xml:space="preserve"> Trabalho de Graduação I</t>
   </si>
   <si>
-    <t>5009972</t>
-  </si>
-  <si>
-    <t>Gilberto Carvalho Coelho</t>
-  </si>
-  <si>
     <t>LOM3063</t>
   </si>
   <si>
@@ -677,12 +683,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Fenômenos de Transporte em Engenharia de Materiais</t>
-  </si>
-  <si>
-    <t>1176388</t>
-  </si>
-  <si>
-    <t>Luiz Tadeu Fernandes Eleno</t>
   </si>
   <si>
     <t>LOM3084</t>
@@ -1321,7 +1321,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D151"/>
+  <dimension ref="A1:D152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1709,87 +1709,93 @@
       <c r="B28" s="2" t="s">
         <v>96</v>
       </c>
+      <c r="C28" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="C30" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D30" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="C31" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D31" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="C33" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D33" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="C35" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D35" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="C36" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D36" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1802,24 +1808,24 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="C39" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D39" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1832,217 +1838,211 @@
     </row>
     <row r="41" spans="1:4">
       <c r="C41" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D41" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>90</v>
+      <c r="C43" t="s">
+        <v>127</v>
+      </c>
+      <c r="D43" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>130</v>
+        <v>90</v>
       </c>
     </row>
     <row r="45" spans="1:4">
-      <c r="C45" t="s">
-        <v>119</v>
-      </c>
-      <c r="D45" t="s">
-        <v>120</v>
+      <c r="A45" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>110</v>
+      <c r="C46" t="s">
+        <v>121</v>
+      </c>
+      <c r="D46" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="47" spans="1:4">
-      <c r="C47" t="s">
-        <v>133</v>
-      </c>
-      <c r="D47" t="s">
-        <v>134</v>
+      <c r="A47" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>134</v>
+      <c r="C48" t="s">
+        <v>137</v>
+      </c>
+      <c r="D48" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="D49" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
     </row>
     <row r="51" spans="1:4">
-      <c r="C51" t="s">
-        <v>141</v>
-      </c>
-      <c r="D51" t="s">
-        <v>142</v>
+      <c r="A51" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" t="s">
         <v>145</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="D52" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="53" spans="1:4">
-      <c r="C53" t="s">
-        <v>133</v>
-      </c>
-      <c r="D53" t="s">
-        <v>134</v>
+      <c r="A53" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>146</v>
+      <c r="C54" t="s">
+        <v>137</v>
+      </c>
+      <c r="D54" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="D55" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="C57" t="s">
-        <v>153</v>
-      </c>
-      <c r="D57" t="s">
-        <v>154</v>
+      <c r="A57" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C58" s="2" t="s">
+      <c r="C58" t="s">
         <v>157</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="D58" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2054,32 +2054,32 @@
         <v>160</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>121</v>
+        <v>161</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>122</v>
+        <v>162</v>
       </c>
     </row>
     <row r="60" spans="1:4">
-      <c r="C60" t="s">
-        <v>133</v>
-      </c>
-      <c r="D60" t="s">
-        <v>134</v>
+      <c r="A60" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>164</v>
+      <c r="C61" t="s">
+        <v>137</v>
+      </c>
+      <c r="D61" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -2090,31 +2090,31 @@
         <v>166</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>113</v>
+        <v>167</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>114</v>
+        <v>168</v>
       </c>
     </row>
     <row r="63" spans="1:4">
-      <c r="C63" t="s">
-        <v>167</v>
-      </c>
-      <c r="D63" t="s">
-        <v>168</v>
+      <c r="A63" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="64" spans="1:4">
-      <c r="A64" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="C64" s="2" t="s">
+      <c r="C64" t="s">
         <v>171</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="D64" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2126,32 +2126,32 @@
         <v>174</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="66" spans="1:4">
-      <c r="C66" t="s">
-        <v>119</v>
-      </c>
-      <c r="D66" t="s">
-        <v>120</v>
+      <c r="A66" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>178</v>
+      <c r="C67" t="s">
+        <v>121</v>
+      </c>
+      <c r="D67" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -2176,18 +2176,18 @@
         <v>184</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>181</v>
@@ -2198,16 +2198,16 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -2218,10 +2218,10 @@
         <v>192</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>189</v>
+        <v>97</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>190</v>
+        <v>98</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -2232,10 +2232,10 @@
         <v>194</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>171</v>
+        <v>97</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>172</v>
+        <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -2246,10 +2246,10 @@
         <v>196</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -2260,120 +2260,120 @@
         <v>198</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>109</v>
+        <v>175</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>110</v>
+        <v>176</v>
       </c>
     </row>
     <row r="76" spans="1:4">
-      <c r="C76" t="s">
-        <v>171</v>
-      </c>
-      <c r="D76" t="s">
-        <v>172</v>
+      <c r="A76" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="77" spans="1:4">
-      <c r="A77" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>110</v>
+      <c r="C77" t="s">
+        <v>175</v>
+      </c>
+      <c r="D77" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="78" spans="1:4">
-      <c r="C78" t="s">
-        <v>133</v>
-      </c>
-      <c r="D78" t="s">
-        <v>134</v>
+      <c r="A78" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="79" spans="1:4">
-      <c r="A79" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>110</v>
+      <c r="C79" t="s">
+        <v>137</v>
+      </c>
+      <c r="D79" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="80" spans="1:4">
-      <c r="C80" t="s">
-        <v>133</v>
-      </c>
-      <c r="D80" t="s">
-        <v>134</v>
+      <c r="A80" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="81" spans="1:4">
-      <c r="A81" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>122</v>
+      <c r="C81" t="s">
+        <v>137</v>
+      </c>
+      <c r="D81" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="82" spans="1:4">
-      <c r="C82" t="s">
-        <v>133</v>
-      </c>
-      <c r="D82" t="s">
-        <v>134</v>
+      <c r="A82" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="83" spans="1:4">
-      <c r="A83" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>122</v>
+      <c r="C83" t="s">
+        <v>137</v>
+      </c>
+      <c r="D83" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="84" spans="1:4">
-      <c r="C84" t="s">
-        <v>133</v>
-      </c>
-      <c r="D84" t="s">
-        <v>134</v>
+      <c r="A84" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="85" spans="1:4">
-      <c r="A85" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>122</v>
+      <c r="C85" t="s">
+        <v>137</v>
+      </c>
+      <c r="D85" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -2384,10 +2384,10 @@
         <v>210</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -2398,408 +2398,414 @@
         <v>212</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="88" spans="1:4">
-      <c r="C88" t="s">
+      <c r="A88" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="D88" t="s">
+      <c r="B88" s="2" t="s">
         <v>214</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="C89" t="s">
-        <v>93</v>
+        <v>215</v>
       </c>
       <c r="D89" t="s">
-        <v>94</v>
+        <v>216</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="C90" t="s">
-        <v>215</v>
+        <v>93</v>
       </c>
       <c r="D90" t="s">
-        <v>216</v>
+        <v>94</v>
       </c>
     </row>
     <row r="91" spans="1:4">
-      <c r="A91" s="2" t="s">
+      <c r="C91" t="s">
         <v>217</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="D91" t="s">
         <v>218</v>
       </c>
-      <c r="C91" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>122</v>
-      </c>
     </row>
     <row r="92" spans="1:4">
-      <c r="C92" t="s">
-        <v>133</v>
-      </c>
-      <c r="D92" t="s">
-        <v>134</v>
+      <c r="A92" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="93" spans="1:4">
-      <c r="A93" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>222</v>
+      <c r="C93" t="s">
+        <v>137</v>
+      </c>
+      <c r="D93" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="B95" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="C94" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4">
-      <c r="C95" t="s">
+      <c r="C95" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="C96" t="s">
         <v>93</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D96" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
-      <c r="A96" s="2" t="s">
+    <row r="97" spans="1:4">
+      <c r="A97" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="B97" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="C96" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4">
-      <c r="C97" t="s">
-        <v>145</v>
-      </c>
-      <c r="D97" t="s">
-        <v>146</v>
+      <c r="C97" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="C98" t="s">
-        <v>119</v>
+        <v>149</v>
       </c>
       <c r="D98" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="C99" t="s">
+        <v>121</v>
+      </c>
+      <c r="D99" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="C100" t="s">
         <v>89</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D100" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
-      <c r="A100" s="2" t="s">
+    <row r="101" spans="1:4">
+      <c r="A101" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B101" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="C100" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4">
-      <c r="C101" t="s">
-        <v>181</v>
-      </c>
-      <c r="D101" t="s">
-        <v>182</v>
+      <c r="C101" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="102" spans="1:4">
       <c r="C102" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="D102" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
     </row>
     <row r="103" spans="1:4">
       <c r="C103" t="s">
+        <v>181</v>
+      </c>
+      <c r="D103" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="C104" t="s">
         <v>93</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D104" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
-      <c r="A104" s="2" t="s">
+    <row r="105" spans="1:4">
+      <c r="A105" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="B105" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="C104" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4">
-      <c r="C105" t="s">
+      <c r="C105" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D105" t="s">
+      <c r="D105" s="2" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="106" spans="1:4">
       <c r="C106" t="s">
-        <v>189</v>
+        <v>111</v>
       </c>
       <c r="D106" t="s">
-        <v>190</v>
+        <v>112</v>
       </c>
     </row>
     <row r="107" spans="1:4">
-      <c r="A107" s="2" t="s">
+      <c r="C107" t="s">
+        <v>97</v>
+      </c>
+      <c r="D107" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="B108" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="C107" s="2" t="s">
+      <c r="C108" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="C109" t="s">
         <v>181</v>
       </c>
-      <c r="D107" s="2" t="s">
+      <c r="D109" t="s">
         <v>182</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4">
-      <c r="C108" t="s">
-        <v>177</v>
-      </c>
-      <c r="D108" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4">
-      <c r="A109" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D109" s="2" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>119</v>
+        <v>175</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>120</v>
+        <v>176</v>
       </c>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="D112" s="2" t="s">
-        <v>190</v>
+        <v>238</v>
       </c>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>163</v>
+        <v>97</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>164</v>
+        <v>98</v>
       </c>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>129</v>
+        <v>167</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>130</v>
+        <v>168</v>
       </c>
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="B115" s="2" t="s">
+      <c r="B116" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="C115" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D115" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4">
-      <c r="C116" t="s">
-        <v>171</v>
-      </c>
-      <c r="D116" t="s">
-        <v>172</v>
+      <c r="C116" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="117" spans="1:4">
-      <c r="A117" s="2" t="s">
+      <c r="C117" t="s">
+        <v>175</v>
+      </c>
+      <c r="D117" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B118" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="C117" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D117" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4">
-      <c r="C118" t="s">
+      <c r="C118" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="C119" t="s">
         <v>249</v>
       </c>
-      <c r="D118" t="s">
+      <c r="D119" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="119" spans="1:4">
-      <c r="A119" s="2" t="s">
+    <row r="120" spans="1:4">
+      <c r="A120" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="B120" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="C119" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D119" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4">
-      <c r="C120" t="s">
-        <v>93</v>
-      </c>
-      <c r="D120" t="s">
-        <v>94</v>
+      <c r="C120" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="121" spans="1:4">
       <c r="C121" t="s">
-        <v>215</v>
+        <v>93</v>
       </c>
       <c r="D121" t="s">
-        <v>216</v>
+        <v>94</v>
       </c>
     </row>
     <row r="122" spans="1:4">
-      <c r="A122" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="C122" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="D122" s="2" t="s">
-        <v>216</v>
+      <c r="C122" t="s">
+        <v>217</v>
+      </c>
+      <c r="D122" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="B123" s="2" t="s">
+      <c r="B124" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="C123" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D123" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4">
-      <c r="C124" t="s">
-        <v>213</v>
-      </c>
-      <c r="D124" t="s">
-        <v>214</v>
+      <c r="C124" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -2811,25 +2817,25 @@
       </c>
     </row>
     <row r="126" spans="1:4">
-      <c r="A126" s="2" t="s">
+      <c r="C126" t="s">
+        <v>217</v>
+      </c>
+      <c r="D126" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="B126" s="2" t="s">
+      <c r="B127" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="C126" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D126" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4">
-      <c r="C127" t="s">
-        <v>213</v>
-      </c>
-      <c r="D127" t="s">
-        <v>214</v>
+      <c r="C127" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -2841,253 +2847,247 @@
       </c>
     </row>
     <row r="129" spans="1:4">
-      <c r="A129" s="2" t="s">
+      <c r="C129" t="s">
+        <v>217</v>
+      </c>
+      <c r="D129" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B129" s="2" t="s">
+      <c r="B130" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="C129" s="2" t="s">
+      <c r="C130" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D129" s="2" t="s">
+      <c r="D130" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="130" spans="1:4">
-      <c r="C130" t="s">
-        <v>103</v>
-      </c>
-      <c r="D130" t="s">
-        <v>104</v>
-      </c>
-    </row>
     <row r="131" spans="1:4">
-      <c r="A131" s="2" t="s">
+      <c r="C131" t="s">
+        <v>105</v>
+      </c>
+      <c r="D131" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="B131" s="2" t="s">
+      <c r="B132" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="C131" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D131" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4">
-      <c r="C132" t="s">
+      <c r="C132" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="C133" t="s">
         <v>249</v>
       </c>
-      <c r="D132" t="s">
+      <c r="D133" t="s">
         <v>250</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4">
-      <c r="A133" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="B133" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="C133" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="D133" s="2" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D140" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="B140" s="2" t="s">
+      <c r="B141" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="C140" s="2" t="s">
+      <c r="C141" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="D140" s="2" t="s">
+      <c r="D141" s="2" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="141" spans="1:4">
-      <c r="C141" t="s">
+    <row r="142" spans="1:4">
+      <c r="C142" t="s">
         <v>291</v>
       </c>
-      <c r="D141" t="s">
+      <c r="D142" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="142" spans="1:4">
-      <c r="A142" s="2" t="s">
+    <row r="143" spans="1:4">
+      <c r="A143" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="B142" s="2" t="s">
+      <c r="B143" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="C142" s="2" t="s">
+      <c r="C143" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="D142" s="2" t="s">
+      <c r="D143" s="2" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="143" spans="1:4">
-      <c r="C143" t="s">
+    <row r="144" spans="1:4">
+      <c r="C144" t="s">
         <v>295</v>
       </c>
-      <c r="D143" t="s">
+      <c r="D144" t="s">
         <v>296</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4">
-      <c r="A144" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="B144" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="C144" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="D144" s="2" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>301</v>
+        <v>265</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>302</v>
+        <v>266</v>
       </c>
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>269</v>
+        <v>301</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>270</v>
+        <v>302</v>
       </c>
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C148" s="2" t="s">
         <v>281</v>
@@ -3098,10 +3098,10 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C149" s="2" t="s">
         <v>281</v>
@@ -3112,29 +3112,43 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>314</v>
+        <v>282</v>
       </c>
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D151" s="2" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4">
+      <c r="A152" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="B151" s="2" t="s">
+      <c r="B152" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="C151" s="2" t="s">
+      <c r="C152" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="D151" s="2" t="s">
+      <c r="D152" s="2" t="s">
         <v>318</v>
       </c>
     </row>

</xml_diff>